<commit_message>
Se modifica AndroidMobile para hacer uso de excel
</commit_message>
<xml_diff>
--- a/dataInput/LineasIOSMiCuenta.xlsx
+++ b/dataInput/LineasIOSMiCuenta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Personal\dataInput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A674155\Code\Personal\dataInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ADFB7A9F-16C0-459B-A913-F0F063090AF4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7B805F5B-0FAB-4BAF-8A3A-231F11A34330}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,11 +551,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -664,7 +664,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <v>1145642605</v>
+        <v>1164590129</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>